<commit_message>
- Changed components description in BOM - Fixed issues in Layout - Fixed issues in Schematic - Generated new documentation
</commit_message>
<xml_diff>
--- a/Released/BOM/H0FR8.xlsx
+++ b/Released/BOM/H0FR8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hexabitz\H0FR8x-Hardware\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C871D12-C73D-4492-97BB-798EC2413E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335618D2-E5D9-4623-82C9-B90112D8C743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,9 +100,6 @@
     <t>FB1</t>
   </si>
   <si>
-    <t>Ind chip Bead Multi-Layer 30 ohms 25% 100MHZ Ferrite 1,5A 0603Punched paper T/R</t>
-  </si>
-  <si>
     <t xml:space="preserve">TDK </t>
   </si>
   <si>
@@ -217,11 +214,6 @@
     <t>GRM21BC81E475KA12L</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Murata GRM21BC81E475KA12L
-Multilayer Ceramic Capacitor, GRM Series, 4.7 - F, - 10%, X6S, 25 V, 0805 [2012 Metric</t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
@@ -285,9 +277,6 @@
     <t>C9</t>
   </si>
   <si>
-    <t>450V 10nF X7T 20% 0805 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
-  </si>
-  <si>
     <t>https://octopart.com/c2012x7t2w103m085aa-tdk-28169246</t>
   </si>
   <si>
@@ -297,15 +286,9 @@
     <t>https://octopart.com/c0603c102k8ractu-kemet-9143718</t>
   </si>
   <si>
-    <t>Cap Ceramic 0.001uF 10V X7R 10% SMD 0603 125C Paper T/R</t>
-  </si>
-  <si>
     <t>C0603C103K5RACTU</t>
   </si>
   <si>
-    <t>Capacitor, Multilayer, Ceramic, 50V, 10%, X7R, 15% Tc, 0.01Uf, Surface Mount, 0603</t>
-  </si>
-  <si>
     <t>https://octopart.com/c0603c103k5ractu-kemet-133094</t>
   </si>
   <si>
@@ -315,9 +298,6 @@
     <t>C2012X7T2W473K125AA</t>
   </si>
   <si>
-    <t>450V 47nF X7T 10% 0805 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
-  </si>
-  <si>
     <t>https://octopart.com/c2012x7t2w473k125aa-tdk-26013889</t>
   </si>
   <si>
@@ -327,9 +307,6 @@
     <t>https://octopart.com/cdsod323-t03sc-bourns-10487153</t>
   </si>
   <si>
-    <t>CDSOD323-TxxSC - TVS Diode Series</t>
-  </si>
-  <si>
     <t>DIODE SCHOTTKY 100V 150MA SOD123</t>
   </si>
   <si>
@@ -360,18 +337,12 @@
     <t>AC0603FR-131KL</t>
   </si>
   <si>
-    <t>Res Thick Film 0603 1K Ohm 1% 0.1W(1/10W) ±100ppm/°C Pad SMD T/R Automotive AEC-Q200</t>
-  </si>
-  <si>
     <t>https://octopart.com/ac0603fr-131kl-yageo-73876229</t>
   </si>
   <si>
     <t>RC0402FR-07100RL</t>
   </si>
   <si>
-    <t>SMD Chip Resistor, 100 Ohm, 1%, 62.5 mW, 0402 [1005 Metric], Thick Film, General Purpose</t>
-  </si>
-  <si>
     <t>https://octopart.com/rc0402fr-07100rl-yageo-40952494</t>
   </si>
   <si>
@@ -384,9 +355,6 @@
     <t xml:space="preserve">Panasonic </t>
   </si>
   <si>
-    <t>SMD Chip Resistor, 100 Ohm, 5%, 500 mW, 0805 [2012 Metric], Thick Film, Anti-Surge</t>
-  </si>
-  <si>
     <t>https://octopart.com/erj-p06j101v-panasonic-39989292</t>
   </si>
   <si>
@@ -396,9 +364,6 @@
     <t>ERJ-P06J391V</t>
   </si>
   <si>
-    <t>Res Thick Film 0805 390 Ohm 5% 1/4W ±200ppm/°C Molded SMD SMD Punched Carrier T/R</t>
-  </si>
-  <si>
     <t>https://octopart.com/erj-p06j391v-panasonic-39814046</t>
   </si>
   <si>
@@ -411,9 +376,6 @@
     <t>Royal Ohm</t>
   </si>
   <si>
-    <t>Thick Film Resistors - SMD RMC 0603 1/10W 5% T/R-5000</t>
-  </si>
-  <si>
     <t>https://octopart.com/0603waj0333t5e-royal+ohm-127861239</t>
   </si>
   <si>
@@ -423,9 +385,6 @@
     <t>RC0603FR-073K3L</t>
   </si>
   <si>
-    <t>Res General Purpose Thick Film 0603 3.3K Ohm 1% 1/10W ±100ppm/°C Molded SMD Paper T/R</t>
-  </si>
-  <si>
     <t>https://octopart.com/rc0603fr-073k3l-yageo-40011875</t>
   </si>
   <si>
@@ -435,9 +394,6 @@
     <t>RC0603FR-0747RL</t>
   </si>
   <si>
-    <t>SMD Chip Resistor, 47 Ohm  1%, 100 mW, 0603 [1608 Metric], Thick Film, General Purpose</t>
-  </si>
-  <si>
     <t>https://octopart.com/rc0603fr-0747rl-yageo-40952917</t>
   </si>
   <si>
@@ -447,21 +403,12 @@
     <t>ERJ-P06J104V</t>
   </si>
   <si>
-    <t>Res Thick Film 0805 100K Ohm 5% 0.25W ±200ppm/°C Molded SMD Punched Carrier T/R</t>
-  </si>
-  <si>
     <t>https://octopart.com/erj-p06j104v-panasonic-39853801</t>
   </si>
   <si>
     <t>R13</t>
   </si>
   <si>
-    <t xml:space="preserve">	ERJ-P06J152V</t>
-  </si>
-  <si>
-    <t>Res Thick Film 0805 1.5K Ohm 5% 0.25W ±200ppm/°C Molded SMD Punched Carrier T/R</t>
-  </si>
-  <si>
     <t>https://octopart.com/erj-p06j152v-panasonic-39824464</t>
   </si>
   <si>
@@ -526,6 +473,57 @@
   </si>
   <si>
     <t>AC_MAINS, LOAD</t>
+  </si>
+  <si>
+    <t>RES 1K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RES 100 OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RES SMD 100 OHM 5% 1/2W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 390 OHM 5% 1/2W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD RMC 33k OHM 0603 1/10W 5%</t>
+  </si>
+  <si>
+    <t>RES 3.3K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RES 47 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RES SMD 100K OHM 5% 1/2W 0805</t>
+  </si>
+  <si>
+    <t>ERJ-P06J152V</t>
+  </si>
+  <si>
+    <t>RES SMD 1.5K OHM 5% 1/2W 0805</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 25V X6S 0805</t>
+  </si>
+  <si>
+    <t>CAP CER 1000PF 10V X7R 0603</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 450V X7T 0805</t>
+  </si>
+  <si>
+    <t>CAP CER 0.047UF 450V X7T 0805</t>
+  </si>
+  <si>
+    <t>FERRITE BEAD 30 OHM 0603 1LN</t>
+  </si>
+  <si>
+    <t>TVS DIODE 3.3VWM 10.9VC SOD323</t>
   </si>
 </sst>
 </file>
@@ -775,6 +773,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -795,9 +796,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1176,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1221,11 +1219,11 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="23">
         <v>0</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.4">
@@ -1233,16 +1231,16 @@
         <v>9</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="25"/>
+      <c r="D5" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.4">
@@ -1250,14 +1248,14 @@
         <v>10</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="28"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="29"/>
       <c r="G6" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.4">
@@ -1282,19 +1280,19 @@
     </row>
     <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>36</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9" s="18">
         <v>1</v>
@@ -1302,7 +1300,7 @@
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>17</v>
@@ -1322,19 +1320,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B11" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="D11" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="E11" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="F11" s="18">
         <v>1</v>
@@ -1342,39 +1340,39 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B12" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>70</v>
-      </c>
       <c r="D12" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>71</v>
-      </c>
       <c r="F12" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>107</v>
+        <v>146</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F13" s="18">
         <v>1</v>
@@ -1382,79 +1380,79 @@
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="28" x14ac:dyDescent="0.35">
-      <c r="A15" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" s="17" t="s">
+      <c r="D16" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="21" t="s">
         <v>109</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="F15" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="28" x14ac:dyDescent="0.35">
-      <c r="A16" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="F16" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A17" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>120</v>
       </c>
       <c r="F17" s="18">
         <v>1</v>
@@ -1462,99 +1460,99 @@
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="F18" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="F19" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" s="17" t="s">
+      <c r="D21" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="21" t="s">
         <v>122</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="F18" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A19" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="F19" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A20" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="F20" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A21" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="F21" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="F22" s="18">
         <v>1</v>
@@ -1562,19 +1560,19 @@
     </row>
     <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F23" s="18">
         <v>4</v>
@@ -1582,39 +1580,39 @@
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="56" x14ac:dyDescent="0.35">
-      <c r="A25" s="17" t="s">
-        <v>77</v>
-      </c>
       <c r="B25" s="17" t="s">
-        <v>60</v>
+        <v>156</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F25" s="18">
         <v>1</v>
@@ -1622,39 +1620,39 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>86</v>
+        <v>157</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F26" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>88</v>
+        <v>158</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F27" s="18">
         <v>1</v>
@@ -1662,19 +1660,19 @@
     </row>
     <row r="28" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A28" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="21" t="s">
         <v>80</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>83</v>
       </c>
       <c r="F28" s="18">
         <v>1</v>
@@ -1682,39 +1680,39 @@
     </row>
     <row r="29" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>92</v>
+        <v>160</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F29" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B30" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="E30" s="21" t="s">
         <v>23</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>24</v>
       </c>
       <c r="F30" s="18">
         <v>1</v>
@@ -1722,19 +1720,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="17" t="s">
+      <c r="D31" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="21" t="s">
         <v>52</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E31" s="21" t="s">
-        <v>53</v>
       </c>
       <c r="F31" s="18">
         <v>1</v>
@@ -1742,19 +1740,19 @@
     </row>
     <row r="32" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="29" t="s">
-        <v>96</v>
+        <v>55</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>162</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F32" s="18">
         <v>1</v>
@@ -1762,19 +1760,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="17" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F33" s="18">
         <v>2</v>
@@ -1782,19 +1780,19 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="F34" s="18">
         <v>1</v>
@@ -1802,19 +1800,19 @@
     </row>
     <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="E35" s="21" t="s">
         <v>49</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" s="21" t="s">
-        <v>50</v>
       </c>
       <c r="F35" s="18">
         <v>1</v>
@@ -1822,19 +1820,19 @@
     </row>
     <row r="36" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F36" s="18">
         <v>1</v>
@@ -1842,19 +1840,19 @@
     </row>
     <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="17" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="F37" s="18">
         <v>1</v>
@@ -1862,19 +1860,19 @@
     </row>
     <row r="38" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="F38" s="18">
         <v>1</v>
@@ -1882,19 +1880,19 @@
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="17" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="D39" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="F39" s="18">
         <v>2</v>
@@ -1902,19 +1900,19 @@
     </row>
     <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="C40" s="17" t="s">
         <v>28</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>29</v>
       </c>
       <c r="D40" s="17" t="s">
         <v>15</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F40" s="18">
         <v>1</v>

</xml_diff>

<commit_message>
- Changed layout - Rearranged components in BOM
</commit_message>
<xml_diff>
--- a/Released/BOM/H0FR8.xlsx
+++ b/Released/BOM/H0FR8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hexabitz\H0FR8x-Hardware\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCDD0E5-8346-4DA9-A683-1E1D3DF7DF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8525EC5-ABA7-4E7B-B356-2BA2D714A8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15480" yWindow="-2670" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -832,7 +832,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2349859</xdr:colOff>
+      <xdr:colOff>2353034</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>16192</xdr:rowOff>
     </xdr:to>
@@ -1174,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1778,41 +1778,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B35" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C35" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D35" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="E34" s="21" t="s">
+      <c r="E35" s="21" t="s">
         <v>127</v>
-      </c>
-      <c r="F34" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" s="21" t="s">
-        <v>49</v>
       </c>
       <c r="F35" s="18">
         <v>1</v>
@@ -1926,7 +1926,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E30" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E35" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E34" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="E40" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="E10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="E23" r:id="rId5" xr:uid="{01DF3B85-9108-476B-8AD5-F1F39BFC2F9F}"/>
@@ -1952,7 +1952,7 @@
     <hyperlink ref="E12" r:id="rId25" xr:uid="{F6B1E337-A483-40A0-9050-C273083D7B97}"/>
     <hyperlink ref="E22" r:id="rId26" xr:uid="{EE5508FD-5DAB-4BB7-B56D-E4A767AD62EF}"/>
     <hyperlink ref="E18" r:id="rId27" xr:uid="{B29E5844-88FF-4369-9824-37A3396F9D47}"/>
-    <hyperlink ref="E34" r:id="rId28" xr:uid="{1376F036-7170-4DA5-A231-394AC82E9DD2}"/>
+    <hyperlink ref="E35" r:id="rId28" xr:uid="{1376F036-7170-4DA5-A231-394AC82E9DD2}"/>
     <hyperlink ref="E36" r:id="rId29" xr:uid="{9085BE70-86E3-4F7E-ABED-54706B918EA3}"/>
     <hyperlink ref="E37" r:id="rId30" xr:uid="{EBBBEDD3-0667-4455-9D80-0E660B0C8C71}"/>
     <hyperlink ref="E38" r:id="rId31" xr:uid="{F91FDC10-5AA9-42E6-92B5-348C89D0FD7C}"/>

</xml_diff>

<commit_message>
-The final design, all done.
</commit_message>
<xml_diff>
--- a/Released/BOM/H0FR8.xlsx
+++ b/Released/BOM/H0FR8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hexabitz\H0FR8x-Hardware\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H0FR8x-Hardware\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8525EC5-ABA7-4E7B-B356-2BA2D714A8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79EA92C-90EC-4AA3-8167-551CCFDB72C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15480" yWindow="-2670" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H0FR8" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,33 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Moazen</author>
+  </authors>
+  <commentList>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{E318298C-8ABB-4A39-89A7-B0700B33ADEB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ATS-PCB1074
+(alternative)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="179">
   <si>
     <t>Description</t>
   </si>
@@ -130,9 +155,6 @@
     <t>Hexabitz Modules</t>
   </si>
   <si>
-    <t>U2</t>
-  </si>
-  <si>
     <t>RESET</t>
   </si>
   <si>
@@ -148,9 +170,6 @@
     <t>https://octopart.com/5-146280-1-te+connectivity+%2F+amp-40259676?r=sp</t>
   </si>
   <si>
-    <t>CAP CER 0.1UF 25V X7R 0603</t>
-  </si>
-  <si>
     <t>RES 10K Ohm 1% 0603</t>
   </si>
   <si>
@@ -205,36 +224,15 @@
     <t>D2</t>
   </si>
   <si>
-    <t>https://octopart.com/grm21bc81e475ka12l-murata-10331911?r=sp&amp;s=RY3qZSD8T6mG6TC9CHI5qQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Murata </t>
-  </si>
-  <si>
-    <t>GRM21BC81E475KA12L</t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
-    <t>https://octopart.com/crcw060310k0jneb-vishay+dale-46603268</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vishay </t>
   </si>
   <si>
-    <t>CRCW060310K0JNEB</t>
-  </si>
-  <si>
-    <t>https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp&amp;s=9bS9ASSwSEqMCE9KBEQZ0g</t>
-  </si>
-  <si>
     <t xml:space="preserve">KEMET </t>
   </si>
   <si>
-    <t>C0603C104K8RACTU</t>
-  </si>
-  <si>
     <t>270.0R  Thick Film Resistors - SMD 0603</t>
   </si>
   <si>
@@ -307,21 +305,9 @@
     <t>https://octopart.com/cdsod323-t03sc-bourns-10487153</t>
   </si>
   <si>
-    <t>DIODE SCHOTTKY 100V 150MA SOD123</t>
-  </si>
-  <si>
-    <t>BAT46ZFILM</t>
-  </si>
-  <si>
     <t xml:space="preserve">STMicroelectronics </t>
   </si>
   <si>
-    <t>https://octopart.com/bat46zfilm-stmicroelectronics-658190</t>
-  </si>
-  <si>
-    <t>D3, D4</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
@@ -340,12 +326,6 @@
     <t>https://octopart.com/ac0603fr-131kl-yageo-73876229</t>
   </si>
   <si>
-    <t>RC0402FR-07100RL</t>
-  </si>
-  <si>
-    <t>https://octopart.com/rc0402fr-07100rl-yageo-40952494</t>
-  </si>
-  <si>
     <t>R12</t>
   </si>
   <si>
@@ -388,9 +368,6 @@
     <t>https://octopart.com/rc0603fr-073k3l-yageo-40011875</t>
   </si>
   <si>
-    <t>R9</t>
-  </si>
-  <si>
     <t>RC0603FR-0747RL</t>
   </si>
   <si>
@@ -436,9 +413,6 @@
     <t>U4</t>
   </si>
   <si>
-    <t>TLP184_GR-TPL,SE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Toshiba </t>
   </si>
   <si>
@@ -448,9 +422,6 @@
     <t>https://octopart.com/tlp184%28gr-tpl%2Cse%28t-toshiba-33798875</t>
   </si>
   <si>
-    <t>U5</t>
-  </si>
-  <si>
     <t>V275LA4P</t>
   </si>
   <si>
@@ -478,9 +449,6 @@
     <t>RES 1K OHM 1% 1/10W 0603</t>
   </si>
   <si>
-    <t>RES 100 OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
     <t>RES SMD 100 OHM 5% 1/2W 0805</t>
   </si>
   <si>
@@ -505,9 +473,6 @@
     <t>RES SMD 1.5K OHM 5% 1/2W 0805</t>
   </si>
   <si>
-    <t>CAP CER 4.7UF 25V X6S 0805</t>
-  </si>
-  <si>
     <t>CAP CER 1000PF 10V X7R 0603</t>
   </si>
   <si>
@@ -524,17 +489,125 @@
   </si>
   <si>
     <t>TVS DIODE 3.3VWM 10.9VC SOD323</t>
+  </si>
+  <si>
+    <t>TLP184(GR-TPL,SE</t>
+  </si>
+  <si>
+    <t>MMSZ5225BT1G</t>
+  </si>
+  <si>
+    <t>RC0603FR-0710KL</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rc0603fr-0710kl-yageo-40025538?r=sp</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1 UF 25V 10% X7R 0603</t>
+  </si>
+  <si>
+    <t>CL10B104KA8NNNC</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cl10b104ka8nnnc-samsung-19831573?r=sp</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 16V X7R 0805</t>
+  </si>
+  <si>
+    <t>C0805C475K4RACTU</t>
+  </si>
+  <si>
+    <t>KEMET [VA]</t>
+  </si>
+  <si>
+    <t>https://octopart.com/c0805c475k4ractu-kemet-22859922?r=sp</t>
+  </si>
+  <si>
+    <t>https://octopart.com/mmsz5225bt1g-onsemi-56609</t>
+  </si>
+  <si>
+    <t>onsemi </t>
+  </si>
+  <si>
+    <t>Zener Diode 3 V 500 mW ±5% Surface Mount SOD-123</t>
+  </si>
+  <si>
+    <t>RES 100 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>AC0603FR-13100RL</t>
+  </si>
+  <si>
+    <t>https://octopart.com/ac0603fr-13100rl-yageo-74169481?r=sp</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>RES 100K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RC0603FR-07100KL</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rc0603fr-07100kl-yageo-40946036?r=sp</t>
+  </si>
+  <si>
+    <t>R9, R14</t>
+  </si>
+  <si>
+    <t>Transistor, Bipolar, Si, NPN, General Purpose, VCEO 40VDC, IC 200mA, PD 225mW, SOT-23</t>
+  </si>
+  <si>
+    <t>MMBT3904LT1G</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>https://octopart.com/mmbt3904lt1g-on+semiconductor-3280?r=sp</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Z1, Z2</t>
+  </si>
+  <si>
+    <t>VDR1</t>
+  </si>
+  <si>
+    <t>ATS-PCB1073</t>
+  </si>
+  <si>
+    <t>Heat Sink TO-263 (D²Pak) Copper Top Mount</t>
+  </si>
+  <si>
+    <t>Advanced Thermal Solutions Inc.</t>
+  </si>
+  <si>
+    <t>H_S</t>
+  </si>
+  <si>
+    <t>https://octopart.com/ats-pcb1073-advanced+thermal+solutions-51854777</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -542,7 +615,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -553,28 +626,28 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -595,7 +668,7 @@
     <font>
       <b/>
       <sz val="36"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -612,13 +685,26 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="7"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -628,6 +714,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -767,15 +859,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -796,6 +879,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1171,25 +1263,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.1796875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.81640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.19921875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.796875" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="46" x14ac:dyDescent="1">
+    <row r="2" spans="1:7" ht="45.6" x14ac:dyDescent="0.75">
       <c r="A2" s="6"/>
       <c r="B2" s="15"/>
       <c r="C2" s="8" t="s">
@@ -1200,7 +1292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="12"/>
       <c r="C3" s="2"/>
@@ -1209,7 +1301,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -1219,14 +1311,14 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="20">
         <v>0</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1236,29 +1328,29 @@
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
+      <c r="D5" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="29"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="26"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1278,29 +1370,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>34</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>35</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="20" t="s">
-        <v>36</v>
+      <c r="E9" s="27" t="s">
+        <v>35</v>
       </c>
       <c r="F9" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>17</v>
@@ -1311,610 +1403,670 @@
       <c r="D10" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="27" t="s">
         <v>19</v>
       </c>
       <c r="F10" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="F11" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="F12" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="F15" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="F22" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="D12" s="17" t="s">
+      <c r="B23" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="F24" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="F12" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="F13" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="F14" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="F16" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="F17" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="F18" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="F19" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="F21" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="F22" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="17" t="s">
+      <c r="B26" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="27" t="s">
         <v>73</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>82</v>
       </c>
       <c r="F26" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>158</v>
+        <v>70</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>138</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>84</v>
+        <v>56</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>75</v>
       </c>
       <c r="F27" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>159</v>
+        <v>69</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>139</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="21" t="s">
-        <v>80</v>
+      <c r="E28" s="27" t="s">
+        <v>71</v>
       </c>
       <c r="F28" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>160</v>
+        <v>76</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>140</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="21" t="s">
-        <v>87</v>
+      <c r="E29" s="27" t="s">
+        <v>78</v>
       </c>
       <c r="F29" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="F30" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="F32" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="E33" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="F33" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="C30" s="17" t="s">
+      <c r="B34" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D34" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E34" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="17" t="s">
+      <c r="F34" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" s="17" t="s">
+      <c r="F35" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="F31" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="17" t="s">
+      <c r="B36" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F36" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="F37" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="F38" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="F39" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F40" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="F32" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F33" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="F34" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="E35" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="F35" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A36" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="F36" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="E37" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="F37" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="28" x14ac:dyDescent="0.35">
-      <c r="A38" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="F38" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="B39" s="17" t="s">
+      <c r="E41" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E39" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="F39" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="17" t="s">
+      <c r="D42" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E42" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="F42" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B43" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C43" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D43" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="E43" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F40" s="18">
+      <c r="F43" s="18">
         <v>1</v>
       </c>
     </row>
@@ -1925,40 +2077,41 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E30" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E34" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E40" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E23" r:id="rId5" xr:uid="{01DF3B85-9108-476B-8AD5-F1F39BFC2F9F}"/>
-    <hyperlink ref="E20" r:id="rId6" xr:uid="{9CD624AB-68FA-45A0-BDA6-CACF754DD34A}"/>
-    <hyperlink ref="E24" r:id="rId7" xr:uid="{AE63E577-2AF8-4B24-A43D-F4255BA5FD41}"/>
-    <hyperlink ref="E11" r:id="rId8" xr:uid="{0A412581-708B-4B43-BCE9-F288010C1F6C}"/>
-    <hyperlink ref="E31" r:id="rId9" xr:uid="{301AE570-2045-4255-B607-FD75AE5DA7F8}"/>
-    <hyperlink ref="E25" r:id="rId10" xr:uid="{D0D8A6B6-6D38-4B73-B861-AACA1609CEF8}"/>
-    <hyperlink ref="E9" r:id="rId11" xr:uid="{48762FAB-6BA7-44F3-B66F-9D2208B135F2}"/>
-    <hyperlink ref="E15" r:id="rId12" xr:uid="{D2D372F9-DA4F-43C8-B46D-E866F10E6982}"/>
-    <hyperlink ref="E28" r:id="rId13" xr:uid="{46171F89-C105-4324-9DD8-181FBB0A1DAD}"/>
+    <hyperlink ref="E43" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E42" r:id="rId2" xr:uid="{EBBBEDD3-0667-4455-9D80-0E660B0C8C71}"/>
+    <hyperlink ref="E33" r:id="rId3" xr:uid="{F91FDC10-5AA9-42E6-92B5-348C89D0FD7C}"/>
+    <hyperlink ref="E20" r:id="rId4" xr:uid="{B29E5844-88FF-4369-9824-37A3396F9D47}"/>
+    <hyperlink ref="E25" r:id="rId5" xr:uid="{EE5508FD-5DAB-4BB7-B56D-E4A767AD62EF}"/>
+    <hyperlink ref="E14" r:id="rId6" xr:uid="{F6B1E337-A483-40A0-9050-C273083D7B97}"/>
+    <hyperlink ref="E21" r:id="rId7" xr:uid="{18C8D691-3F4F-4B29-9079-BC7F640B59FE}"/>
+    <hyperlink ref="E23" r:id="rId8" xr:uid="{BDAD3E54-5B15-4A36-82B5-2FF4A8C68DE5}"/>
+    <hyperlink ref="E18" r:id="rId9" xr:uid="{A980DA3B-D798-4A86-A800-07D0AD367C63}"/>
+    <hyperlink ref="E16" r:id="rId10" xr:uid="{5D2AB246-23F6-47D7-887E-E15E7C88151B}"/>
+    <hyperlink ref="E19" r:id="rId11" xr:uid="{FA91E9DA-469C-4BA0-85D2-73EFE6338940}"/>
+    <hyperlink ref="E29" r:id="rId12" xr:uid="{7208AD47-5884-484F-9C71-10726BEE3B30}"/>
+    <hyperlink ref="E27" r:id="rId13" xr:uid="{0C5136B0-D976-4705-870E-B093BB4A114F}"/>
     <hyperlink ref="E26" r:id="rId14" xr:uid="{3C865F83-58D6-4BD7-A832-148C8D077F0F}"/>
-    <hyperlink ref="E27" r:id="rId15" xr:uid="{0C5136B0-D976-4705-870E-B093BB4A114F}"/>
-    <hyperlink ref="E29" r:id="rId16" xr:uid="{7208AD47-5884-484F-9C71-10726BEE3B30}"/>
-    <hyperlink ref="E32" r:id="rId17" xr:uid="{B4BF16DA-318B-45E9-9AAB-D23D175C7E77}"/>
-    <hyperlink ref="E33" r:id="rId18" xr:uid="{2F4690D7-DCBC-4F0F-BE30-B649DF49F06B}"/>
-    <hyperlink ref="E17" r:id="rId19" xr:uid="{FA91E9DA-469C-4BA0-85D2-73EFE6338940}"/>
-    <hyperlink ref="E13" r:id="rId20" xr:uid="{F5BFFEE3-0597-4836-B17A-3E6FFBF8E5DC}"/>
-    <hyperlink ref="E14" r:id="rId21" xr:uid="{5D2AB246-23F6-47D7-887E-E15E7C88151B}"/>
-    <hyperlink ref="E16" r:id="rId22" xr:uid="{A980DA3B-D798-4A86-A800-07D0AD367C63}"/>
-    <hyperlink ref="E21" r:id="rId23" xr:uid="{BDAD3E54-5B15-4A36-82B5-2FF4A8C68DE5}"/>
-    <hyperlink ref="E19" r:id="rId24" xr:uid="{18C8D691-3F4F-4B29-9079-BC7F640B59FE}"/>
-    <hyperlink ref="E12" r:id="rId25" xr:uid="{F6B1E337-A483-40A0-9050-C273083D7B97}"/>
-    <hyperlink ref="E22" r:id="rId26" xr:uid="{EE5508FD-5DAB-4BB7-B56D-E4A767AD62EF}"/>
-    <hyperlink ref="E18" r:id="rId27" xr:uid="{B29E5844-88FF-4369-9824-37A3396F9D47}"/>
-    <hyperlink ref="E35" r:id="rId28" xr:uid="{1376F036-7170-4DA5-A231-394AC82E9DD2}"/>
-    <hyperlink ref="E36" r:id="rId29" xr:uid="{9085BE70-86E3-4F7E-ABED-54706B918EA3}"/>
-    <hyperlink ref="E37" r:id="rId30" xr:uid="{EBBBEDD3-0667-4455-9D80-0E660B0C8C71}"/>
-    <hyperlink ref="E38" r:id="rId31" xr:uid="{F91FDC10-5AA9-42E6-92B5-348C89D0FD7C}"/>
+    <hyperlink ref="E28" r:id="rId15" xr:uid="{46171F89-C105-4324-9DD8-181FBB0A1DAD}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{D2D372F9-DA4F-43C8-B46D-E866F10E6982}"/>
+    <hyperlink ref="E9" r:id="rId17" xr:uid="{48762FAB-6BA7-44F3-B66F-9D2208B135F2}"/>
+    <hyperlink ref="E10" r:id="rId18" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E41" r:id="rId19" xr:uid="{9085BE70-86E3-4F7E-ABED-54706B918EA3}"/>
+    <hyperlink ref="E39" r:id="rId20" xr:uid="{1376F036-7170-4DA5-A231-394AC82E9DD2}"/>
+    <hyperlink ref="E36" r:id="rId21" xr:uid="{B4BF16DA-318B-45E9-9AAB-D23D175C7E77}"/>
+    <hyperlink ref="E35" r:id="rId22" xr:uid="{301AE570-2045-4255-B607-FD75AE5DA7F8}"/>
+    <hyperlink ref="E40" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E34" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E22" r:id="rId25" display="https://octopart.com/crcw060310k0jneb-vishay+dale-46603268" xr:uid="{04CD56C7-7880-4F36-9DE5-09752675F5E5}"/>
+    <hyperlink ref="E32" r:id="rId26" display="https://octopart.com/grm21bc81e475ka12l-murata-10331911?r=sp&amp;s=RY3qZSD8T6mG6TC9CHI5qQ" xr:uid="{2E4DC996-34AB-435A-9A04-8AEA8A4C3B68}"/>
+    <hyperlink ref="E31" r:id="rId27" xr:uid="{D02BF949-2407-4F1C-BE3D-E85630AF0C7E}"/>
+    <hyperlink ref="E30" r:id="rId28" display="https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp&amp;s=9bS9ASSwSEqMCE9KBEQZ0g" xr:uid="{B80A4630-EB28-4ECB-8E65-CCD173D94859}"/>
+    <hyperlink ref="E13" r:id="rId29" xr:uid="{0A412581-708B-4B43-BCE9-F288010C1F6C}"/>
+    <hyperlink ref="E24" r:id="rId30" xr:uid="{308EA33D-1471-4C0F-8B14-CDCED8B1DC11}"/>
+    <hyperlink ref="E12" r:id="rId31" xr:uid="{0D3171A6-6F48-487D-96E0-713AB176A5C9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId32"/>
   <drawing r:id="rId33"/>
+  <legacyDrawing r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>